<commit_message>
MATRIZ DE ANALISIS DE RIESGOS
identificacion de los riesgos del proyecto, plan de contingencia y plan de prevencion
</commit_message>
<xml_diff>
--- a/Estimación PF.xlsx
+++ b/Estimación PF.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\ADMINISTRACION DE SISTEMAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\SI-Super-Pollo-\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="PFSA" sheetId="1" r:id="rId1"/>
@@ -964,31 +964,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -999,7 +980,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1008,6 +1005,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1733,6 +1733,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2025,9 +2073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2042,12 +2090,12 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
@@ -2098,10 +2146,10 @@
         <f t="shared" ref="G3:G7" si="0">B3*F3</f>
         <v>84</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="34"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2135,7 +2183,7 @@
       </c>
       <c r="M4">
         <f>G8*(0.65+(0.01*58))</f>
-        <v>736.77</v>
+        <v>655.59</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2156,11 +2204,11 @@
         <v>6</v>
       </c>
       <c r="F5" s="14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>198</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2213,17 +2261,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="47">
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="34">
         <f>SUM(G3:G7)</f>
-        <v>599</v>
+        <v>533</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2234,10 +2282,10 @@
       <c r="A10" s="17"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="D11" s="35" t="s">
         <v>84</v>
       </c>
@@ -2559,11 +2607,11 @@
       <c r="B23" s="25">
         <v>1</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="27">
         <f>SUM(F13:G22)</f>
         <v>14</v>
@@ -2588,8 +2636,8 @@
       <c r="B24" s="25">
         <v>1</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="I24" s="30" t="s">
         <v>88</v>
       </c>
@@ -2608,8 +2656,8 @@
       <c r="B25" s="25">
         <v>1</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="9"/>
       <c r="I25" s="30" t="s">
         <v>89</v>
@@ -2631,8 +2679,8 @@
       <c r="B26" s="25">
         <v>1</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="9"/>
       <c r="I26" s="30" t="s">
         <v>80</v>
@@ -2655,8 +2703,8 @@
         <f>SUM(B13:B26)</f>
         <v>14</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="I27" s="36" t="s">
         <v>81</v>
       </c>
@@ -6577,30 +6625,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A8:F8"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6613,8 +6661,8 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6851,10 +6899,10 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="39"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="5">
         <f>SUM(C2:C15)</f>
         <v>58</v>
@@ -6883,7 +6931,7 @@
       </c>
       <c r="C19" s="10">
         <f>PFSA!G8*(0.65+(0.01*C16))</f>
-        <v>736.77</v>
+        <v>655.59</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -13769,7 +13817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -13809,7 +13857,7 @@
       </c>
       <c r="E2" s="19">
         <f>PF!C19</f>
-        <v>736.77</v>
+        <v>655.59</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -13854,7 +13902,7 @@
       </c>
       <c r="E5" s="20">
         <f>E2/E3</f>
-        <v>46.048124999999999</v>
+        <v>40.974375000000002</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -13869,7 +13917,7 @@
       </c>
       <c r="E6" s="20">
         <f>E5/E4</f>
-        <v>11.51203125</v>
+        <v>10.24359375</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>